<commit_message>
shorou e 2-2 va 0-1
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\github repository\github repository\arduinotadris\چارت آموزشی\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\Arduino\tadris\چارت آموزشی\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{72805D22-0B5A-41DA-8793-40D57451E100}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10056" windowHeight="7572" tabRatio="878" firstSheet="31" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="486">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1261,7 +1260,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1324,7 +1323,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1334,7 +1333,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1566,16 +1565,22 @@
   <si>
     <t>||</t>
   </si>
+  <si>
+    <t>عملگرهای ریاضی</t>
+  </si>
+  <si>
+    <t>عملگرهای منطقی</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1588,7 +1593,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1602,7 +1607,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1622,7 +1627,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1635,7 +1640,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -2020,26 +2025,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>380</v>
       </c>
@@ -2056,7 +2059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>381</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>155</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>157</v>
       </c>
@@ -2114,7 +2117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>221</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>132</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>222</v>
       </c>
@@ -2250,7 +2253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>293</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>271</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>294</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>373</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>296</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>295</v>
       </c>
@@ -2383,7 +2386,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>185</v>
       </c>
@@ -2397,7 +2400,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:8" ht="19.5" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>158</v>
       </c>
@@ -2408,7 +2411,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>159</v>
       </c>
@@ -2421,7 +2424,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2434,7 +2437,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>372</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>382</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>383</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2499,7 +2502,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -2519,18 +2522,18 @@
         <v>477</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>450</v>
       </c>
       <c r="B32" s="16"/>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -2538,23 +2541,23 @@
         <v>451</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>395</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>306</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>469</v>
       </c>
@@ -2572,48 +2575,48 @@
     <mergeCell ref="A32:B32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی " xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی " xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 " xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C"/>
+    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card"/>
+    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2621,45 +2624,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="5:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>307</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>299</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>308</v>
       </c>
@@ -2701,19 +2704,19 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2721,20 +2724,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>470</v>
       </c>
@@ -2742,44 +2745,44 @@
         <v>471</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>418</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>177</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>411</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>419</v>
       </c>
@@ -2820,7 +2823,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>291</v>
       </c>
@@ -2828,36 +2831,36 @@
         <v>424</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>410</v>
       </c>
@@ -2871,7 +2874,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>177</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>411</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>291</v>
       </c>
@@ -2904,35 +2907,35 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>176</v>
       </c>
@@ -2946,7 +2949,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>177</v>
       </c>
@@ -2958,7 +2961,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -2968,70 +2971,70 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>170</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>171</v>
       </c>
@@ -3055,7 +3058,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>172</v>
       </c>
@@ -3063,36 +3066,36 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>161</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>167</v>
       </c>
@@ -3127,7 +3130,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>162</v>
       </c>
@@ -3136,36 +3139,36 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>186</v>
       </c>
@@ -3180,7 +3183,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>188</v>
@@ -3192,7 +3195,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>189</v>
@@ -3204,7 +3207,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>190</v>
@@ -3214,94 +3217,94 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.77734375" customWidth="1"/>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3309,23 +3312,23 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>325</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>326</v>
       </c>
@@ -3353,36 +3356,36 @@
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>297</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>298</v>
       </c>
@@ -3415,44 +3418,44 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>346</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>347</v>
       </c>
@@ -3495,7 +3498,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>348</v>
       </c>
@@ -3515,7 +3518,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>349</v>
       </c>
@@ -3527,97 +3530,97 @@
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>332</v>
       </c>
@@ -3628,7 +3631,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>333</v>
       </c>
@@ -3636,44 +3639,44 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>267</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>276</v>
       </c>
@@ -3721,7 +3724,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>277</v>
       </c>
@@ -3732,78 +3735,78 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>270</v>
       </c>
@@ -3820,7 +3823,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3831,7 +3834,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>261</v>
       </c>
@@ -3839,19 +3842,19 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3859,21 +3862,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>240</v>
       </c>
@@ -3881,50 +3884,50 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>247</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>244</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3932,24 +3935,24 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
@@ -3963,7 +3966,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>224</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>227</v>
       </c>
@@ -3985,65 +3988,65 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>435</v>
       </c>
@@ -4051,7 +4054,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>436</v>
       </c>
@@ -4059,7 +4062,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>437</v>
       </c>
@@ -4067,40 +4070,40 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -4114,7 +4117,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -4133,44 +4136,44 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>196</v>
       </c>
@@ -4207,7 +4210,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>209</v>
       </c>
@@ -4221,7 +4224,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>200</v>
       </c>
@@ -4229,76 +4232,76 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -4335,57 +4338,57 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>113</v>
       </c>
@@ -4417,7 +4420,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
@@ -4432,7 +4435,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>115</v>
       </c>
@@ -4445,7 +4448,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -4456,36 +4459,36 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -4499,7 +4502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -4513,24 +4516,24 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4538,57 +4541,57 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -4602,7 +4605,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -4616,7 +4619,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -4627,7 +4630,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>106</v>
       </c>
@@ -4635,7 +4638,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>107</v>
       </c>
@@ -4643,19 +4646,19 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4663,23 +4666,23 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>123</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
@@ -4707,7 +4710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>125</v>
       </c>
@@ -4721,7 +4724,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>129</v>
@@ -4733,7 +4736,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>69</v>
@@ -4741,40 +4744,40 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4797,7 +4800,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -4833,7 +4836,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
@@ -4842,47 +4845,47 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F6" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>316</v>
       </c>
@@ -4891,7 +4894,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>177</v>
       </c>
@@ -4899,7 +4902,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>317</v>
       </c>
@@ -4907,7 +4910,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>323</v>
       </c>
@@ -4915,24 +4918,24 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4940,52 +4943,52 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -5014,7 +5017,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -5048,90 +5051,102 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B1" t="s">
         <v>254</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B2" t="s">
         <v>249</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>255</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>256</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>409</v>
       </c>
@@ -5148,35 +5163,35 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>400</v>
       </c>
@@ -5187,7 +5202,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>401</v>
       </c>
@@ -5195,7 +5210,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>177</v>
       </c>
@@ -5203,7 +5218,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>402</v>
       </c>
@@ -5211,7 +5226,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -5219,45 +5234,45 @@
         <v>430</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>400</v>
       </c>
@@ -5268,7 +5283,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>401</v>
       </c>
@@ -5279,7 +5294,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>177</v>
       </c>
@@ -5290,7 +5305,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>402</v>
       </c>
@@ -5301,7 +5316,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
         <v>319</v>
       </c>
@@ -5309,86 +5324,86 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="1" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>460</v>
       </c>
@@ -5399,7 +5414,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -5407,7 +5422,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>461</v>
       </c>
@@ -5415,42 +5430,42 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>439</v>
       </c>
@@ -5467,7 +5482,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>440</v>
       </c>
@@ -5481,7 +5496,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>441</v>
       </c>
@@ -5495,7 +5510,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>442</v>
       </c>
@@ -5505,14 +5520,14 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
takmile matn va code haye 2-2
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="489">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1570,6 +1570,15 @@
   </si>
   <si>
     <t>عملگرهای منطقی</t>
+  </si>
+  <si>
+    <t>define</t>
+  </si>
+  <si>
+    <t>دکمه (ورودی دیجیتال)</t>
+  </si>
+  <si>
+    <t>چشمک زن (خروجی دیجیتال)</t>
   </si>
 </sst>
 </file>
@@ -2028,7 +2037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2119,7 +2130,7 @@
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>488</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>386</v>
@@ -2177,7 +2188,7 @@
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>487</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>388</v>
@@ -4623,6 +4634,9 @@
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
takmile 3-1 va shoroue 8-3
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\github repository\github repository\arduinotadris\چارت آموزشی\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\Arduino\tadris\چارت آموزشی\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE920CFB-3DCB-4B57-89FC-7F65A090B9A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10056" windowHeight="7572" tabRatio="878" firstSheet="28" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1258,7 +1257,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1321,7 +1320,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1331,7 +1330,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1585,12 +1584,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1603,7 +1602,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1617,7 +1616,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1637,7 +1636,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1650,16 +1649,9 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="B Nazanin"/>
-      <charset val="178"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1695,7 +1687,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1714,7 +1706,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2035,26 +2026,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>379</v>
       </c>
@@ -2071,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>380</v>
       </c>
@@ -2091,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>154</v>
       </c>
@@ -2111,7 +2102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>156</v>
       </c>
@@ -2129,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>487</v>
       </c>
@@ -2149,7 +2140,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
@@ -2169,7 +2160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>220</v>
       </c>
@@ -2187,7 +2178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>486</v>
       </c>
@@ -2207,7 +2198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>131</v>
       </c>
@@ -2227,7 +2218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>221</v>
       </c>
@@ -2265,7 +2256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2285,7 +2276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>292</v>
       </c>
@@ -2303,7 +2294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>270</v>
       </c>
@@ -2323,7 +2314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>293</v>
       </c>
@@ -2343,7 +2334,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>372</v>
       </c>
@@ -2360,8 +2351,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
+      <c r="A17" s="14" t="s">
         <v>295</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2380,7 +2371,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>294</v>
       </c>
@@ -2398,7 +2389,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>184</v>
       </c>
@@ -2412,18 +2403,18 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="14" t="s">
+      <c r="C20" t="s">
         <v>477</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>158</v>
       </c>
@@ -2436,7 +2427,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2449,7 +2440,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>371</v>
       </c>
@@ -2457,7 +2448,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2468,7 +2459,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -2476,7 +2467,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2484,7 +2475,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>381</v>
       </c>
@@ -2495,7 +2486,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>382</v>
       </c>
@@ -2506,7 +2497,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2514,7 +2505,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -2525,7 +2516,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -2534,18 +2525,18 @@
         <v>476</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
+      <c r="A32" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="B32" s="16"/>
-    </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+      <c r="B32" s="15"/>
+    </row>
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -2553,23 +2544,23 @@
         <v>450</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>394</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>305</v>
       </c>
@@ -2577,7 +2568,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>468</v>
       </c>
@@ -2587,48 +2578,48 @@
     <mergeCell ref="A32:B32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی " xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی " xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 " xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C"/>
+    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card"/>
+    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2636,45 +2627,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="5:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>306</v>
       </c>
@@ -2688,7 +2679,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>298</v>
       </c>
@@ -2702,7 +2693,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>307</v>
       </c>
@@ -2716,19 +2707,19 @@
         <v>458</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2736,20 +2727,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>469</v>
       </c>
@@ -2757,44 +2748,44 @@
         <v>470</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>417</v>
       </c>
@@ -2805,7 +2796,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>176</v>
       </c>
@@ -2816,7 +2807,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>410</v>
       </c>
@@ -2827,7 +2818,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>418</v>
       </c>
@@ -2835,7 +2826,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>290</v>
       </c>
@@ -2843,36 +2834,36 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>409</v>
       </c>
@@ -2886,7 +2877,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>176</v>
       </c>
@@ -2900,7 +2891,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>410</v>
       </c>
@@ -2911,7 +2902,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>290</v>
       </c>
@@ -2919,35 +2910,35 @@
         <v>456</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -2961,7 +2952,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>176</v>
       </c>
@@ -2973,7 +2964,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>177</v>
       </c>
@@ -2983,70 +2974,70 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>169</v>
       </c>
@@ -3060,7 +3051,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>170</v>
       </c>
@@ -3070,7 +3061,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>171</v>
       </c>
@@ -3078,36 +3069,36 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -3121,7 +3112,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>165</v>
       </c>
@@ -3133,7 +3124,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>166</v>
       </c>
@@ -3142,7 +3133,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>161</v>
       </c>
@@ -3151,36 +3142,36 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -3195,7 +3186,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>187</v>
@@ -3207,7 +3198,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>188</v>
@@ -3219,7 +3210,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>189</v>
@@ -3229,94 +3220,94 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.77734375" customWidth="1"/>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3324,23 +3315,23 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>324</v>
       </c>
@@ -3355,7 +3346,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>325</v>
       </c>
@@ -3368,36 +3359,36 @@
         <v>330</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -3411,7 +3402,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>296</v>
       </c>
@@ -3422,7 +3413,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>297</v>
       </c>
@@ -3430,44 +3421,44 @@
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>345</v>
       </c>
@@ -3490,7 +3481,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>346</v>
       </c>
@@ -3510,7 +3501,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>347</v>
       </c>
@@ -3530,7 +3521,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>348</v>
       </c>
@@ -3542,97 +3533,97 @@
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>331</v>
       </c>
@@ -3643,7 +3634,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>332</v>
       </c>
@@ -3651,44 +3642,44 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>266</v>
       </c>
@@ -3705,7 +3696,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>290</v>
       </c>
@@ -3722,7 +3713,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>275</v>
       </c>
@@ -3736,7 +3727,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>276</v>
       </c>
@@ -3747,78 +3738,78 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>269</v>
       </c>
@@ -3835,7 +3826,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3846,7 +3837,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>260</v>
       </c>
@@ -3854,19 +3845,19 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3874,21 +3865,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>239</v>
       </c>
@@ -3896,50 +3887,50 @@
         <v>240</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>241</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>245</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>246</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>244</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3947,24 +3938,24 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>222</v>
       </c>
@@ -3978,7 +3969,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>223</v>
       </c>
@@ -3992,7 +3983,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>226</v>
       </c>
@@ -4000,65 +3991,65 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>434</v>
       </c>
@@ -4066,7 +4057,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>435</v>
       </c>
@@ -4074,7 +4065,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>436</v>
       </c>
@@ -4082,40 +4073,40 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>209</v>
       </c>
@@ -4129,7 +4120,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -4140,7 +4131,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>211</v>
       </c>
@@ -4148,44 +4139,44 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
@@ -4205,7 +4196,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>195</v>
       </c>
@@ -4222,7 +4213,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -4236,7 +4227,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>199</v>
       </c>
@@ -4244,76 +4235,76 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -4336,7 +4327,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -4350,57 +4341,57 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
@@ -4417,7 +4408,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>112</v>
       </c>
@@ -4432,7 +4423,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>113</v>
       </c>
@@ -4447,7 +4438,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>114</v>
       </c>
@@ -4460,7 +4451,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>115</v>
       </c>
@@ -4471,36 +4462,36 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
@@ -4514,7 +4505,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -4528,24 +4519,24 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4553,57 +4544,57 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>159</v>
       </c>
@@ -4617,7 +4608,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -4631,7 +4622,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -4645,7 +4636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C4" s="2" t="s">
         <v>105</v>
       </c>
@@ -4653,7 +4644,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C5" s="2" t="s">
         <v>106</v>
       </c>
@@ -4661,19 +4652,19 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4681,23 +4672,23 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
@@ -4714,7 +4705,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
@@ -4731,7 +4722,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -4748,7 +4739,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
@@ -4762,7 +4753,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -4772,50 +4763,50 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4835,7 +4826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -4846,7 +4837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -4854,7 +4845,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -4862,47 +4853,47 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>315</v>
       </c>
@@ -4911,7 +4902,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>176</v>
       </c>
@@ -4919,7 +4910,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>316</v>
       </c>
@@ -4927,7 +4918,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>322</v>
       </c>
@@ -4935,24 +4926,24 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4960,52 +4951,52 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -5034,7 +5025,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -5051,7 +5042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -5068,33 +5059,33 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>483</v>
       </c>
@@ -5105,7 +5096,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>484</v>
       </c>
@@ -5116,7 +5107,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>254</v>
       </c>
@@ -5124,7 +5115,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>255</v>
       </c>
@@ -5132,14 +5123,14 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5147,23 +5138,23 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>408</v>
       </c>
@@ -5180,35 +5171,35 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>399</v>
       </c>
@@ -5219,7 +5210,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>400</v>
       </c>
@@ -5227,7 +5218,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>176</v>
       </c>
@@ -5235,7 +5226,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>401</v>
       </c>
@@ -5243,7 +5234,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -5251,45 +5242,45 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>399</v>
       </c>
@@ -5300,7 +5291,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>400</v>
       </c>
@@ -5311,7 +5302,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>176</v>
       </c>
@@ -5322,7 +5313,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>401</v>
       </c>
@@ -5333,7 +5324,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
         <v>318</v>
       </c>
@@ -5341,86 +5332,86 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="1" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>459</v>
       </c>
@@ -5431,7 +5422,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -5439,7 +5430,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>460</v>
       </c>
@@ -5447,42 +5438,42 @@
         <v>398</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>438</v>
       </c>
@@ -5499,7 +5490,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>439</v>
       </c>
@@ -5513,7 +5504,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>440</v>
       </c>
@@ -5527,7 +5518,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>441</v>
       </c>
@@ -5537,14 +5528,14 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>378</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
takmile motaghayerha (static moonde)
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" firstSheet="34" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" firstSheet="25" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="491">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1579,6 +1579,12 @@
   </si>
   <si>
     <t>دیود</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>static</t>
   </si>
 </sst>
 </file>
@@ -2029,7 +2035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4283,8 +4291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4352,6 +4360,16 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
@@ -5134,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
shoroue lcd ta payane ketabkhaneh
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\github repository\github repository\arduinotadris\چارت آموزشی\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\Arduino\tadris\چارت آموزشی\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D8059C-879A-48F5-8B2B-4B24E4655453}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10056" windowHeight="7572" tabRatio="878" firstSheet="25" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" firstSheet="21" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -738,9 +737,6 @@
     <t>clear</t>
   </si>
   <si>
-    <t xml:space="preserve">set curser </t>
-  </si>
-  <si>
     <t xml:space="preserve">print </t>
   </si>
   <si>
@@ -1243,7 +1239,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1306,7 +1302,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1316,7 +1312,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1572,16 +1568,19 @@
   <si>
     <t>const</t>
   </si>
+  <si>
+    <t>setCursor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1594,7 +1593,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1608,7 +1607,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1628,7 +1627,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1641,7 +1640,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -2018,31 +2017,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>152</v>
@@ -2054,15 +2053,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -2074,15 +2073,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -2094,13 +2093,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
@@ -2112,15 +2111,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>151</v>
@@ -2132,15 +2131,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -2152,13 +2151,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
@@ -2170,15 +2169,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
@@ -2190,15 +2189,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>16</v>
@@ -2210,33 +2209,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>26</v>
@@ -2248,15 +2247,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>29</v>
@@ -2268,13 +2267,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>32</v>
@@ -2286,15 +2285,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>35</v>
@@ -2306,15 +2305,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>38</v>
@@ -2326,12 +2325,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>41</v>
@@ -2343,15 +2342,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>44</v>
@@ -2363,31 +2362,31 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>180</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>89</v>
@@ -2395,174 +2394,174 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C23" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C24" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C27" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A28" s="1" t="s">
-        <v>377</v>
-      </c>
       <c r="B28" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C28" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C30" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B32" s="15"/>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -2570,48 +2569,48 @@
     <mergeCell ref="A32:B32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی " xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی " xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 " xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C"/>
+    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card"/>
+    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2619,99 +2618,99 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="5:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2719,145 +2718,145 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B1" t="s">
         <v>464</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -2866,71 +2865,71 @@
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="D3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>171</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2956,7 +2955,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
@@ -2966,70 +2965,70 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>165</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>166</v>
       </c>
@@ -3053,7 +3052,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>167</v>
       </c>
@@ -3061,36 +3060,36 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
@@ -3101,10 +3100,10 @@
         <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>161</v>
       </c>
@@ -3113,10 +3112,10 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>162</v>
       </c>
@@ -3125,7 +3124,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -3134,36 +3133,36 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>181</v>
       </c>
@@ -3178,7 +3177,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>183</v>
@@ -3190,7 +3189,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>184</v>
@@ -3202,7 +3201,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>185</v>
@@ -3212,94 +3211,94 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.77734375" customWidth="1"/>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3307,518 +3306,518 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="2" t="s">
+      <c r="F3" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>326</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>329</v>
       </c>
-      <c r="C1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>327</v>
       </c>
-      <c r="B2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B3" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B12" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3826,30 +3825,30 @@
         <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="B4" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3857,72 +3856,72 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A3" s="6" t="s">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A4" s="6" t="s">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A5" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A7" s="6" t="s">
-        <v>239</v>
-      </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3930,24 +3929,24 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>217</v>
       </c>
@@ -3955,13 +3954,13 @@
         <v>219</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>218</v>
       </c>
@@ -3969,136 +3968,136 @@
         <v>220</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>221</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="B9" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
         <v>429</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="12" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
-        <v>431</v>
-      </c>
       <c r="B3" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -4109,10 +4108,10 @@
         <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -4123,7 +4122,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -4131,44 +4130,44 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4182,13 +4181,13 @@
         <v>199</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>191</v>
       </c>
@@ -4202,10 +4201,10 @@
         <v>200</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>203</v>
       </c>
@@ -4219,7 +4218,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>195</v>
       </c>
@@ -4227,71 +4226,71 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -4311,10 +4310,10 @@
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -4325,60 +4324,60 @@
         <v>140</v>
       </c>
       <c r="G2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4395,7 +4394,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -4410,12 +4409,12 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>116</v>
@@ -4425,12 +4424,12 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>117</v>
@@ -4438,7 +4437,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>111</v>
       </c>
@@ -4449,34 +4448,36 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -4504,24 +4505,24 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4529,57 +4530,57 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>155</v>
       </c>
@@ -4590,7 +4591,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -4601,43 +4602,43 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4645,23 +4646,23 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>118</v>
       </c>
@@ -4678,7 +4679,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -4695,7 +4696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
@@ -4706,13 +4707,13 @@
         <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
@@ -4726,7 +4727,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -4736,50 +4737,50 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4799,7 +4800,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -4810,7 +4811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -4818,7 +4819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -4826,97 +4827,97 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A3" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="B3" s="13" t="s">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
-      <c r="A4" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="B4" s="13" t="s">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4924,52 +4925,52 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -4998,112 +4999,112 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
       <c r="B3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" t="s">
         <v>476</v>
       </c>
-      <c r="C3" t="s">
-        <v>477</v>
-      </c>
       <c r="F3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>248</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="B2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>249</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5111,32 +5112,32 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>87</v>
@@ -5148,371 +5149,371 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
       <c r="F9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="B2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B4" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B2" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.5">
-      <c r="A4" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="B5" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.5">
-      <c r="B5" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="1" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C1" t="s">
         <v>456</v>
       </c>
-      <c r="C1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B3" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B2" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>437</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>459</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>438</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>460</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="12" t="s">
-        <v>436</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
servo ta sare 180 va 360
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" firstSheet="21" activeTab="28"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878" firstSheet="6" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView rightToLeft="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2915,13 +2915,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
     <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
@@ -3929,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Display Modules added to excel
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\github repository\github repository\arduinotadris\چارت آموزشی\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\Arduino\tadris\چارت آموزشی\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F716F5-8BBA-4312-A98F-5D27E4108EA6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="10056" windowHeight="7572" tabRatio="878" firstSheet="21" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="7575" tabRatio="878"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="491">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1237,7 +1236,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1300,7 +1299,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1310,7 +1309,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1569,16 +1568,34 @@
   <si>
     <t>setCursor</t>
   </si>
+  <si>
+    <t>ماژول ها و مباحث اضافه</t>
+  </si>
+  <si>
+    <t>NEXTION</t>
+  </si>
+  <si>
+    <t>نمایشگرها</t>
+  </si>
+  <si>
+    <t>OLED ( I2C, SPI )</t>
+  </si>
+  <si>
+    <t>GLCD ( I2C, SPI , Parallel )</t>
+  </si>
+  <si>
+    <t>TFT ( SPI , Parallel )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1591,7 +1608,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1605,7 +1622,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1625,7 +1642,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1638,7 +1655,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1676,7 +1693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1701,6 +1718,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2015,26 +2036,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>372</v>
       </c>
@@ -2051,7 +2072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>373</v>
       </c>
@@ -2071,7 +2092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>150</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
@@ -2109,7 +2130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>480</v>
       </c>
@@ -2129,7 +2150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
@@ -2149,7 +2170,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2167,7 +2188,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>479</v>
       </c>
@@ -2187,7 +2208,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>127</v>
       </c>
@@ -2207,7 +2228,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
@@ -2245,7 +2266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2265,7 +2286,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>285</v>
       </c>
@@ -2283,7 +2304,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>263</v>
       </c>
@@ -2303,7 +2324,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>286</v>
       </c>
@@ -2323,7 +2344,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>365</v>
       </c>
@@ -2340,7 +2361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>288</v>
       </c>
@@ -2360,7 +2381,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>287</v>
       </c>
@@ -2378,7 +2399,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>180</v>
       </c>
@@ -2392,7 +2413,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>153</v>
       </c>
@@ -2403,7 +2424,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>154</v>
       </c>
@@ -2416,7 +2437,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2429,7 +2450,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>364</v>
       </c>
@@ -2437,7 +2458,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2448,7 +2469,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -2456,7 +2477,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2464,7 +2485,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>374</v>
       </c>
@@ -2475,7 +2496,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>375</v>
       </c>
@@ -2486,7 +2507,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2494,7 +2515,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -2505,7 +2526,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -2514,42 +2535,48 @@
         <v>469</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>442</v>
       </c>
       <c r="B32" s="15"/>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A37" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="16" t="s">
+        <v>485</v>
+      </c>
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.45">
+      <c r="A38" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>387</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>298</v>
       </c>
@@ -2557,58 +2584,94 @@
         <v>444</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>461</v>
       </c>
     </row>
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C48" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="B49" t="s">
+        <v>487</v>
+      </c>
+      <c r="C49" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="C50" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="C51" t="s">
+        <v>471</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A36:B36"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی " xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی " xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 " xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C"/>
+    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card"/>
+    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2616,45 +2679,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="5:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>299</v>
       </c>
@@ -2668,7 +2731,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -2682,7 +2745,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>300</v>
       </c>
@@ -2696,19 +2759,19 @@
         <v>451</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2716,20 +2779,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>462</v>
       </c>
@@ -2737,44 +2800,44 @@
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>410</v>
       </c>
@@ -2785,7 +2848,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2796,7 +2859,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>403</v>
       </c>
@@ -2807,7 +2870,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>411</v>
       </c>
@@ -2815,7 +2878,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>283</v>
       </c>
@@ -2823,36 +2886,36 @@
         <v>416</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>402</v>
       </c>
@@ -2866,7 +2929,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2880,7 +2943,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>403</v>
       </c>
@@ -2891,7 +2954,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>283</v>
       </c>
@@ -2899,35 +2962,35 @@
         <v>449</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>171</v>
       </c>
@@ -2941,7 +3004,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2953,7 +3016,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
@@ -2963,70 +3026,70 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" customWidth="1"/>
+    <col min="1" max="1" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>165</v>
       </c>
@@ -3040,7 +3103,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>166</v>
       </c>
@@ -3050,7 +3113,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>167</v>
       </c>
@@ -3058,36 +3121,36 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
@@ -3101,7 +3164,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>161</v>
       </c>
@@ -3113,7 +3176,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>162</v>
       </c>
@@ -3122,7 +3185,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -3131,36 +3194,36 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>181</v>
       </c>
@@ -3175,7 +3238,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>183</v>
@@ -3187,7 +3250,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>184</v>
@@ -3199,7 +3262,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>185</v>
@@ -3209,94 +3272,94 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.77734375" customWidth="1"/>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3304,23 +3367,23 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>317</v>
       </c>
@@ -3335,7 +3398,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>318</v>
       </c>
@@ -3348,36 +3411,36 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -3391,7 +3454,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3402,7 +3465,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3410,44 +3473,44 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>338</v>
       </c>
@@ -3470,7 +3533,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>339</v>
       </c>
@@ -3490,7 +3553,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>340</v>
       </c>
@@ -3510,7 +3573,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>341</v>
       </c>
@@ -3522,97 +3585,97 @@
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="64.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>324</v>
       </c>
@@ -3623,7 +3686,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>325</v>
       </c>
@@ -3631,44 +3694,44 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>259</v>
       </c>
@@ -3685,7 +3748,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>283</v>
       </c>
@@ -3702,7 +3765,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>268</v>
       </c>
@@ -3716,7 +3779,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>269</v>
       </c>
@@ -3727,78 +3790,78 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>262</v>
       </c>
@@ -3815,7 +3878,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3826,7 +3889,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>253</v>
       </c>
@@ -3834,19 +3897,19 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3854,21 +3917,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.88671875" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>232</v>
       </c>
@@ -3876,50 +3939,50 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>234</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>238</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3927,24 +3990,24 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>217</v>
       </c>
@@ -3958,7 +4021,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>218</v>
       </c>
@@ -3972,70 +4035,70 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>427</v>
       </c>
@@ -4043,7 +4106,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>428</v>
       </c>
@@ -4051,7 +4114,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>429</v>
       </c>
@@ -4059,40 +4122,40 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -4106,7 +4169,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -4117,7 +4180,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -4125,44 +4188,44 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4182,7 +4245,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>191</v>
       </c>
@@ -4199,7 +4262,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>203</v>
       </c>
@@ -4213,7 +4276,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>195</v>
       </c>
@@ -4221,71 +4284,71 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -4308,7 +4371,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -4322,57 +4385,57 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4389,7 +4452,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -4404,7 +4467,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -4419,7 +4482,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
@@ -4432,7 +4495,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>111</v>
       </c>
@@ -4443,36 +4506,36 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -4486,7 +4549,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -4500,24 +4563,24 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4525,57 +4588,57 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>155</v>
       </c>
@@ -4586,7 +4649,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -4597,7 +4660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -4608,7 +4671,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>483</v>
       </c>
@@ -4616,24 +4679,24 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4641,23 +4704,23 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>118</v>
       </c>
@@ -4674,7 +4737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -4691,7 +4754,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
@@ -4708,7 +4771,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
@@ -4722,7 +4785,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -4732,50 +4795,50 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4795,7 +4858,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -4806,7 +4869,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -4814,7 +4877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -4822,47 +4885,47 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>308</v>
       </c>
@@ -4871,7 +4934,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>172</v>
       </c>
@@ -4879,7 +4942,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>309</v>
       </c>
@@ -4887,7 +4950,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>315</v>
       </c>
@@ -4895,24 +4958,24 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4920,52 +4983,52 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -4994,7 +5057,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -5011,7 +5074,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -5028,33 +5091,33 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>476</v>
       </c>
@@ -5065,7 +5128,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>477</v>
       </c>
@@ -5076,7 +5139,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>247</v>
       </c>
@@ -5084,7 +5147,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>248</v>
       </c>
@@ -5092,14 +5155,14 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5107,24 +5170,24 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>401</v>
       </c>
@@ -5144,35 +5207,35 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
       <c r="F9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>392</v>
       </c>
@@ -5183,7 +5246,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>393</v>
       </c>
@@ -5191,7 +5254,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
@@ -5199,7 +5262,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
@@ -5207,7 +5270,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -5215,45 +5278,45 @@
         <v>422</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>392</v>
       </c>
@@ -5264,7 +5327,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>393</v>
       </c>
@@ -5275,7 +5338,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
@@ -5286,7 +5349,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
@@ -5297,7 +5360,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
         <v>311</v>
       </c>
@@ -5305,86 +5368,86 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.77734375" customWidth="1"/>
-    <col min="4" max="4" width="33.21875" customWidth="1"/>
+    <col min="1" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>452</v>
       </c>
@@ -5395,7 +5458,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -5403,7 +5466,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>453</v>
       </c>
@@ -5411,42 +5474,42 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>431</v>
       </c>
@@ -5463,7 +5526,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>432</v>
       </c>
@@ -5477,7 +5540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>433</v>
       </c>
@@ -5491,7 +5554,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>434</v>
       </c>
@@ -5501,14 +5564,14 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some changes in excel
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\github repository\github repository\arduinotadris\چارت آموزشی\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\M\Arduino\tadris\چارت آموزشی\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5DF00-2080-4047-BFFF-11515999C372}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="878" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" tabRatio="878" firstSheet="33" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="494">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -1237,7 +1236,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1300,7 +1299,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1310,7 +1309,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
+        <rFont val="Times New Roman"/>
         <family val="1"/>
         <scheme val="major"/>
       </rPr>
@@ -1593,16 +1592,19 @@
   <si>
     <t>Serial.available()</t>
   </si>
+  <si>
+    <t xml:space="preserve"> if else</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1615,7 +1617,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1629,7 +1631,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1649,7 +1651,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -1662,7 +1664,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -2043,26 +2045,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="41.1015625" customWidth="1"/>
-    <col min="3" max="3" width="25.47265625" customWidth="1"/>
+    <col min="2" max="2" width="41.125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="19.26171875" customWidth="1"/>
-    <col min="6" max="6" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.26171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>372</v>
       </c>
@@ -2079,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>373</v>
       </c>
@@ -2099,7 +2101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>150</v>
       </c>
@@ -2119,7 +2121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>152</v>
       </c>
@@ -2137,7 +2139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>480</v>
       </c>
@@ -2157,7 +2159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>79</v>
       </c>
@@ -2177,7 +2179,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2195,7 +2197,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>479</v>
       </c>
@@ -2215,7 +2217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>127</v>
       </c>
@@ -2235,7 +2237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2253,7 +2255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
@@ -2273,7 +2275,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2293,7 +2295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>285</v>
       </c>
@@ -2311,7 +2313,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>263</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>286</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>365</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>288</v>
       </c>
@@ -2388,7 +2390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>287</v>
       </c>
@@ -2406,7 +2408,7 @@
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>180</v>
       </c>
@@ -2420,7 +2422,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>153</v>
       </c>
@@ -2431,7 +2433,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>154</v>
       </c>
@@ -2444,7 +2446,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2457,7 +2459,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>364</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2476,7 +2478,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -2484,7 +2486,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>374</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>375</v>
       </c>
@@ -2514,7 +2516,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>13</v>
       </c>
@@ -2533,7 +2535,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
@@ -2542,24 +2544,24 @@
         <v>469</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>442</v>
       </c>
       <c r="B32" s="16"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>485</v>
       </c>
       <c r="B36" s="17"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
         <v>47</v>
       </c>
@@ -2567,23 +2569,23 @@
         <v>443</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>387</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>298</v>
       </c>
@@ -2591,12 +2593,12 @@
         <v>444</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>489</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>486</v>
       </c>
@@ -2615,7 +2617,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
         <v>488</v>
       </c>
@@ -2623,7 +2625,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>490</v>
       </c>
@@ -2637,48 +2639,48 @@
     <mergeCell ref="A36:B36"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی " xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی " xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 " xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A7" location="'4 سریال قسمت اول'!A1" display="سریال قسمت 1"/>
+    <hyperlink ref="A4" location="'1 معرفی آردینو '!A1" display="معرفی آردینو"/>
+    <hyperlink ref="A5" location="'2 چشمک زن '!A1" display="چشمک زن"/>
+    <hyperlink ref="A6" location="'3 ترانزیستو و رله '!A1" display="ترانزیستور و رله ( مفهوم مدار تغذیه و کنترل)"/>
+    <hyperlink ref="A8" location="'5 دکمه'!A1" display="دکمه"/>
+    <hyperlink ref="A9" location="'6 انواع متغیر ها'!A1" display="انواع متغیر"/>
+    <hyperlink ref="A10" location="'7 کیپد'!A1" display="کی پد"/>
+    <hyperlink ref="A11" location="'8 سریال قسمت دوم'!A1" display="سریال قسمت 2"/>
+    <hyperlink ref="A12" location="'9نمایشگر کاراکتری'!A1" display="نمایشگر کاراکتری"/>
+    <hyperlink ref="A13" location="'10 انالوگ مقاومت متغیر'!A1" display="آنالوگ مقاومت متغیر و جوی استیک"/>
+    <hyperlink ref="A14" location="'11 انالوگ دماسنجی'!A1" display="آنالوگ دماسنجی "/>
+    <hyperlink ref="A15" location="'12 آنالوگ نور سنجی'!A1" display="آنالوگ نورسنجی"/>
+    <hyperlink ref="A18" location="'15 آنالوگ رنگ سنجی'!A1" display="آنالوگ رنگ سنجی "/>
+    <hyperlink ref="A16" location="'13سریال قسمت سوم'!A1" display="سریال قسمت سوم"/>
+    <hyperlink ref="A17" location="'14 PWM,RGB'!A1" display="PWM , RGB"/>
+    <hyperlink ref="B6" location="'تمرین فصل 1'!A1" display="تمرین فصل 1"/>
+    <hyperlink ref="B9" location="'تمرین فصل 2'!A1" display="تمرین فصل 2"/>
+    <hyperlink ref="B12" location="'تمرین فصل 3'!A1" display="تمرین فصل 3"/>
+    <hyperlink ref="B15" location="'تمرین فصل 4'!A1" display="تمرین فصل 4"/>
+    <hyperlink ref="B18" location="'تمرین فصل 5'!A1" display="تمرین فصل 5"/>
+    <hyperlink ref="A19" location="'16 معرفی موتورها'!A1" display="معرفی موتورها"/>
+    <hyperlink ref="A20" location="'17 موتور دی سی یک'!A1" display="موتور دی سی یک"/>
+    <hyperlink ref="A21" location="'18 موتور دی سی دو'!A1" display="موتور دی سی دو"/>
+    <hyperlink ref="A22" location="'19 سرو'!A1" display="سرو"/>
+    <hyperlink ref="A23" location="'20 استپ'!A1" display="استپر موتور"/>
+    <hyperlink ref="A24" location="'21 براشلس'!A1" display="براشلس"/>
+    <hyperlink ref="A27" location="'22 فاصله سنجی اولتراسونیک'!A1" display="فاصله سنجی اولتراسونیک"/>
+    <hyperlink ref="A1" location="'پیش نیاز الکتریکی'!A1" display="پیش نیاز"/>
+    <hyperlink ref="A2" location="'پیش نیاز برنامه نویسی'!A1" display="پیش نیاز برنامه نویسی"/>
+    <hyperlink ref="A3" location="'مدار منطقی'!A1" display="مدار منطقی"/>
+    <hyperlink ref="B3" location="'تمرین فصل 0'!A1" display="تمرین فصل 0 "/>
+    <hyperlink ref="A31" location="' 28 EEPROM'!A1" display="EEPROM"/>
+    <hyperlink ref="A29" location="' 26 I2C '!A1" display="I2C"/>
+    <hyperlink ref="B21" location="'تمرین فصل 6-1'!A1" display="تمرین فصل 6"/>
+    <hyperlink ref="A28" location="'23 فاصله سنجی آی آر'!A1" display="فاصله سنجی آی آر"/>
+    <hyperlink ref="A25" location="'24 شافت انکودر'!A1" display="شافت انکودر"/>
+    <hyperlink ref="A26" location="'25 روتاری انکودر'!A1" display="روتاری انکودر"/>
+    <hyperlink ref="B28" location="'تمرین فصل 7'!A1" display="تمرین فصل 7"/>
+    <hyperlink ref="A30" location="'27 SPI'!A1" display="SPI"/>
+    <hyperlink ref="A44" location="'30 Tone'!A1" display="Tone (تولید صدا)"/>
+    <hyperlink ref="A43" location="'32 SD Card'!A1" display="SD Card"/>
+    <hyperlink ref="B24" location="'تمرین فصل 6-2'!A1" display="تمرین فصل 6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2686,45 +2688,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="5:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="E10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.62890625" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>299</v>
       </c>
@@ -2738,7 +2740,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
@@ -2752,7 +2754,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>300</v>
       </c>
@@ -2766,19 +2768,19 @@
         <v>451</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C8" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2786,20 +2788,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.734375" customWidth="1"/>
-    <col min="2" max="2" width="43.62890625" customWidth="1"/>
+    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>462</v>
       </c>
@@ -2807,44 +2809,44 @@
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.26171875" customWidth="1"/>
+    <col min="1" max="1" width="18.25" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>410</v>
       </c>
@@ -2855,7 +2857,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>403</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>411</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>283</v>
       </c>
@@ -2893,36 +2895,36 @@
         <v>416</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="D11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.734375" customWidth="1"/>
-    <col min="3" max="3" width="13.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.47265625" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>402</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>403</v>
       </c>
@@ -2961,7 +2963,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>283</v>
       </c>
@@ -2969,35 +2971,35 @@
         <v>449</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.62890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.47265625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>171</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>172</v>
       </c>
@@ -3023,7 +3025,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
@@ -3033,70 +3035,70 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.734375" customWidth="1"/>
+    <col min="1" max="1" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.89453125" customWidth="1"/>
+    <col min="1" max="1" width="11.875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>165</v>
       </c>
@@ -3110,7 +3112,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>166</v>
       </c>
@@ -3120,7 +3122,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>167</v>
       </c>
@@ -3128,36 +3130,36 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.47265625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>161</v>
       </c>
@@ -3183,7 +3185,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>162</v>
       </c>
@@ -3192,7 +3194,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
@@ -3201,36 +3203,36 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.734375" customWidth="1"/>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>181</v>
       </c>
@@ -3245,7 +3247,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>183</v>
@@ -3257,7 +3259,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>184</v>
@@ -3269,7 +3271,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>185</v>
@@ -3279,94 +3281,94 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="D12" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="10" spans="4:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.734375" customWidth="1"/>
+    <col min="1" max="1" width="80.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3374,23 +3376,23 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.62890625" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.734375" customWidth="1"/>
-    <col min="4" max="4" width="17.62890625" customWidth="1"/>
-    <col min="5" max="5" width="51.62890625" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="51.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>317</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>318</v>
       </c>
@@ -3418,36 +3420,36 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.26171875" customWidth="1"/>
-    <col min="2" max="2" width="19.734375" customWidth="1"/>
-    <col min="3" max="3" width="16.734375" customWidth="1"/>
-    <col min="4" max="4" width="24.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -3472,7 +3474,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>290</v>
       </c>
@@ -3480,42 +3482,44 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="C11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1015625" customWidth="1"/>
-    <col min="2" max="2" width="27.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.3671875" customWidth="1"/>
-    <col min="5" max="5" width="31.89453125" customWidth="1"/>
-    <col min="6" max="6" width="28.26171875" customWidth="1"/>
-    <col min="7" max="7" width="32.1015625" customWidth="1"/>
+    <col min="4" max="4" width="29.375" customWidth="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1"/>
+    <col min="6" max="6" width="28.25" customWidth="1"/>
+    <col min="7" max="7" width="32.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>338</v>
       </c>
@@ -3538,7 +3542,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>339</v>
       </c>
@@ -3558,7 +3562,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>340</v>
       </c>
@@ -3578,7 +3582,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>341</v>
       </c>
@@ -3590,97 +3594,97 @@
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="64.47265625" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.734375" customWidth="1"/>
-    <col min="3" max="3" width="26.89453125" customWidth="1"/>
-    <col min="4" max="4" width="26.62890625" customWidth="1"/>
-    <col min="5" max="5" width="25.734375" customWidth="1"/>
+    <col min="1" max="1" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>324</v>
       </c>
@@ -3691,7 +3695,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>325</v>
       </c>
@@ -3699,44 +3703,44 @@
         <v>328</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.47265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="28.1015625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.3671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.26171875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.62890625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>259</v>
       </c>
@@ -3753,7 +3757,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>283</v>
       </c>
@@ -3770,7 +3774,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>268</v>
       </c>
@@ -3784,7 +3788,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>269</v>
       </c>
@@ -3795,78 +3799,78 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="1">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="1">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="1">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="1">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="1">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="1">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="1">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.2" x14ac:dyDescent="1">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="C15" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.47265625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.26171875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.75" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>262</v>
       </c>
@@ -3883,7 +3887,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3894,7 +3898,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>253</v>
       </c>
@@ -3902,19 +3906,19 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.2" x14ac:dyDescent="1">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3922,21 +3926,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.89453125" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="1" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>232</v>
       </c>
@@ -3944,50 +3948,50 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="2" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>234</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>238</v>
       </c>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="4" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="5" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="9" spans="1:2" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="B9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3995,24 +3999,24 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.3671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.89453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.62890625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.1015625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.89453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.875" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>217</v>
       </c>
@@ -4026,7 +4030,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>218</v>
       </c>
@@ -4040,70 +4044,70 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="1">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="1">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="1">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="1">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>427</v>
       </c>
@@ -4111,7 +4115,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>428</v>
       </c>
@@ -4119,7 +4123,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>429</v>
       </c>
@@ -4127,40 +4131,40 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.47265625" customWidth="1"/>
-    <col min="2" max="2" width="34.47265625" customWidth="1"/>
-    <col min="3" max="3" width="30.26171875" customWidth="1"/>
-    <col min="4" max="4" width="46.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="30.25" customWidth="1"/>
+    <col min="4" max="4" width="46.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -4174,7 +4178,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -4185,7 +4189,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -4193,7 +4197,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -4201,44 +4205,44 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.3671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.26171875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.1015625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.47265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.62890625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="38.625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4258,7 +4262,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>191</v>
       </c>
@@ -4275,7 +4279,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="1">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>203</v>
       </c>
@@ -4289,7 +4293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>195</v>
       </c>
@@ -4297,71 +4301,71 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="22.2" x14ac:dyDescent="1">
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.734375" customWidth="1"/>
-    <col min="2" max="2" width="17.89453125" customWidth="1"/>
-    <col min="3" max="3" width="17.734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="B6" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.62890625" customWidth="1"/>
-    <col min="3" max="3" width="16.3671875" customWidth="1"/>
-    <col min="4" max="4" width="5.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.47265625" customWidth="1"/>
+    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -4384,7 +4388,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -4398,57 +4402,57 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.47265625" customWidth="1"/>
-    <col min="5" max="5" width="21.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>107</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -4480,7 +4484,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>109</v>
       </c>
@@ -4495,7 +4499,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
@@ -4508,7 +4512,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>111</v>
       </c>
@@ -4519,36 +4523,36 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3671875" customWidth="1"/>
-    <col min="4" max="4" width="12.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>141</v>
       </c>
@@ -4562,7 +4566,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -4576,24 +4580,24 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="C13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4601,57 +4605,57 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.734375" customWidth="1"/>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="B7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.3671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.3671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.47265625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.3671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.1015625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>155</v>
       </c>
@@ -4662,7 +4666,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -4673,7 +4677,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>85</v>
       </c>
@@ -4684,7 +4688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>483</v>
       </c>
@@ -4692,24 +4696,24 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D5" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="C6" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.2" x14ac:dyDescent="1">
+    <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="B11" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4717,23 +4721,23 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26171875" customWidth="1"/>
-    <col min="3" max="3" width="14.734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.47265625" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>118</v>
       </c>
@@ -4750,7 +4754,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -4767,7 +4771,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
@@ -4784,7 +4788,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>62</v>
       </c>
@@ -4798,7 +4802,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -4808,50 +4812,50 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="B13" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.100000000000001" x14ac:dyDescent="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.89453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.47265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.47265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.47265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -4871,7 +4875,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
@@ -4882,7 +4886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="1">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E3" s="2" t="s">
         <v>57</v>
       </c>
@@ -4890,7 +4894,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>58</v>
       </c>
@@ -4898,47 +4902,47 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="1">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G7" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="22.2" x14ac:dyDescent="1">
+    <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="C10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.734375" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>308</v>
       </c>
@@ -4947,7 +4951,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="2" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>172</v>
       </c>
@@ -4955,7 +4959,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>309</v>
       </c>
@@ -4963,7 +4967,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>315</v>
       </c>
@@ -4971,24 +4975,24 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4996,52 +5000,52 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1015625" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="C4" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.47265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -5070,7 +5074,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -5087,7 +5091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -5104,33 +5108,33 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="G7" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>476</v>
       </c>
@@ -5140,42 +5144,54 @@
       <c r="C1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>477</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>493</v>
       </c>
       <c r="C2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>247</v>
       </c>
       <c r="C3" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>248</v>
       </c>
       <c r="C4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5183,24 +5199,24 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.62890625" customWidth="1"/>
-    <col min="4" max="4" width="11.47265625" customWidth="1"/>
-    <col min="5" max="5" width="11.26171875" customWidth="1"/>
-    <col min="6" max="6" width="10.62890625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.6" x14ac:dyDescent="1.25">
+    <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>401</v>
       </c>
@@ -5220,35 +5236,35 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
       <c r="F9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="F9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" customWidth="1"/>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>392</v>
       </c>
@@ -5259,7 +5275,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>393</v>
       </c>
@@ -5267,7 +5283,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
@@ -5275,7 +5291,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
@@ -5283,7 +5299,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -5291,45 +5307,45 @@
         <v>422</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1015625" customWidth="1"/>
-    <col min="2" max="2" width="16.47265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.734375" customWidth="1"/>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.100000000000001" x14ac:dyDescent="1">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>392</v>
       </c>
@@ -5340,7 +5356,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="1">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>393</v>
       </c>
@@ -5351,7 +5367,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="1">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
@@ -5362,7 +5378,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="1">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
@@ -5373,7 +5389,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="1">
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
         <v>311</v>
       </c>
@@ -5381,86 +5397,86 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="E9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.3671875" customWidth="1"/>
+    <col min="1" max="1" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.734375" customWidth="1"/>
-    <col min="3" max="3" width="41.734375" customWidth="1"/>
-    <col min="4" max="4" width="33.26171875" customWidth="1"/>
+    <col min="1" max="2" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="41.75" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>452</v>
       </c>
@@ -5471,7 +5487,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -5479,7 +5495,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>453</v>
       </c>
@@ -5487,42 +5503,42 @@
         <v>391</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D10" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.47265625" customWidth="1"/>
-    <col min="2" max="2" width="29.89453125" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.89453125" customWidth="1"/>
-    <col min="5" max="5" width="36.734375" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
+    <col min="5" max="5" width="36.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>431</v>
       </c>
@@ -5539,7 +5555,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>432</v>
       </c>
@@ -5553,7 +5569,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>433</v>
       </c>
@@ -5567,7 +5583,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.3" x14ac:dyDescent="1.05">
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>434</v>
       </c>
@@ -5577,14 +5593,14 @@
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
         <v>371</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D9" location="Sheet1!A1" display="صفحه اصلی"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
eslahe bakhshe keypade excel
</commit_message>
<xml_diff>
--- a/چارت آموزشی/آردوینو.xlsx
+++ b/چارت آموزشی/آردوینو.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" tabRatio="878" firstSheet="33" activeTab="41"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" tabRatio="878" firstSheet="23" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="492">
   <si>
     <t>چشمک زن</t>
   </si>
@@ -798,12 +798,6 @@
   </si>
   <si>
     <t>ریختن اعداد در ارایه و نمایش در سریال</t>
-  </si>
-  <si>
-    <t>کد ال ای دی فشاری (case)</t>
-  </si>
-  <si>
-    <t>کد ال ای دی وضعیتی(case)</t>
   </si>
   <si>
     <t xml:space="preserve">if </t>
@@ -2049,7 +2043,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView rightToLeft="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2066,10 +2060,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>152</v>
@@ -2083,13 +2077,13 @@
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -2106,10 +2100,10 @@
         <v>150</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -2127,7 +2121,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
@@ -2141,13 +2135,13 @@
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>151</v>
@@ -2164,10 +2158,10 @@
         <v>79</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>13</v>
@@ -2185,7 +2179,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
@@ -2199,13 +2193,13 @@
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
@@ -2222,10 +2216,10 @@
         <v>127</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>16</v>
@@ -2243,13 +2237,13 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
@@ -2260,10 +2254,10 @@
         <v>216</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>26</v>
@@ -2280,10 +2274,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>29</v>
@@ -2297,11 +2291,11 @@
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>32</v>
@@ -2315,13 +2309,13 @@
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>35</v>
@@ -2335,13 +2329,13 @@
     </row>
     <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>38</v>
@@ -2355,10 +2349,10 @@
     </row>
     <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C16" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>41</v>
@@ -2372,13 +2366,13 @@
     </row>
     <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>44</v>
@@ -2392,19 +2386,19 @@
     </row>
     <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -2414,7 +2408,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>89</v>
@@ -2428,7 +2422,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2438,10 +2432,10 @@
         <v>154</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2451,20 +2445,20 @@
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C23" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.45">
@@ -2472,10 +2466,10 @@
         <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C24" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.45">
@@ -2483,7 +2477,7 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
@@ -2491,29 +2485,29 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C27" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2521,7 +2515,7 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.45">
@@ -2529,10 +2523,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C30" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.45">
@@ -2541,18 +2535,18 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B32" s="16"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B36" s="17"/>
     </row>
@@ -2566,7 +2560,7 @@
         <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
@@ -2581,56 +2575,56 @@
     </row>
     <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C48" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B49" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C49" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C50" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C51" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -2699,7 +2693,7 @@
   <sheetData>
     <row r="10" spans="5:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2728,54 +2722,54 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="C1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
         <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C8" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2803,25 +2797,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2848,13 +2842,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="C1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -2862,42 +2856,42 @@
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D11" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2926,7 +2920,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -2935,7 +2929,7 @@
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -2943,37 +2937,37 @@
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" t="s">
         <v>404</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>406</v>
-      </c>
-      <c r="D2" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="D3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3037,7 +3031,7 @@
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3063,17 +3057,17 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3132,7 +3126,7 @@
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3170,7 +3164,7 @@
         <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -3182,7 +3176,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -3205,7 +3199,7 @@
     </row>
     <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3283,7 +3277,7 @@
     </row>
     <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D12" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3306,7 +3300,7 @@
   <sheetData>
     <row r="10" spans="4:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3333,37 +3327,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3394,35 +3388,35 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3454,42 +3448,42 @@
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C11" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3521,75 +3515,75 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>354</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
@@ -3599,7 +3593,7 @@
     </row>
     <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3626,37 +3620,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3686,31 +3680,31 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3742,106 +3736,106 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C15" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3872,19 +3866,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -3895,25 +3889,25 @@
         <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -3986,7 +3980,7 @@
     </row>
     <row r="9" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4056,7 +4050,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -4086,7 +4080,7 @@
     </row>
     <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4109,26 +4103,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.45">
@@ -4137,7 +4131,7 @@
     </row>
     <row r="7" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D7" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4175,7 +4169,7 @@
         <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4202,17 +4196,17 @@
         <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4227,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -4255,9 +4249,6 @@
       <c r="D1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="F1" s="2" t="s">
         <v>212</v>
       </c>
@@ -4275,9 +4266,6 @@
       <c r="D2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -4303,7 +4291,7 @@
     </row>
     <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4336,7 +4324,7 @@
     </row>
     <row r="6" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4424,7 +4412,7 @@
     </row>
     <row r="13" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4525,7 +4513,7 @@
     </row>
     <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4592,7 +4580,7 @@
     </row>
     <row r="13" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4624,7 +4612,7 @@
     </row>
     <row r="7" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4682,7 +4670,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
@@ -4690,7 +4678,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>83</v>
@@ -4708,7 +4696,7 @@
     </row>
     <row r="11" spans="1:4" ht="22.5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4782,7 +4770,7 @@
         <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>77</v>
@@ -4824,7 +4812,7 @@
     </row>
     <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4916,7 +4904,7 @@
     </row>
     <row r="10" spans="1:7" ht="22.5" x14ac:dyDescent="0.45">
       <c r="C10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4944,7 +4932,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>43</v>
@@ -4956,38 +4944,38 @@
         <v>172</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>309</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5019,7 +5007,7 @@
     </row>
     <row r="4" spans="1:3" ht="22.5" x14ac:dyDescent="0.2">
       <c r="C4" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5079,13 +5067,13 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H2" t="s">
         <v>101</v>
@@ -5096,13 +5084,13 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C3" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H3" t="s">
         <v>102</v>
@@ -5110,7 +5098,7 @@
     </row>
     <row r="7" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="G7" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5125,8 +5113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5136,13 +5124,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D1" t="s">
         <v>128</v>
@@ -5150,10 +5138,10 @@
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C2" t="s">
         <v>242</v>
@@ -5164,10 +5152,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -5175,10 +5163,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
         <v>131</v>
@@ -5186,7 +5174,7 @@
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5218,13 +5206,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>87</v>
@@ -5238,7 +5226,7 @@
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.2">
       <c r="F9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5266,21 +5254,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -5288,15 +5276,15 @@
         <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.45">
@@ -5304,22 +5292,22 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5347,24 +5335,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>395</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
@@ -5372,49 +5360,49 @@
         <v>172</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B5" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5440,17 +5428,17 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5478,13 +5466,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B1" t="s">
         <v>452</v>
       </c>
-      <c r="B1" t="s">
-        <v>454</v>
-      </c>
       <c r="C1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5492,25 +5480,25 @@
         <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D10" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5540,30 +5528,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>57</v>
@@ -5571,31 +5559,31 @@
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D4" s="12"/>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
       <c r="D9" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>